<commit_message>
Different noise figure, maybe more based in reality
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000"/>
+    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -782,6 +782,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,9 +818,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,31 +827,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1142,7 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1275,15 +1275,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
@@ -1300,10 +1300,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="62"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1330,8 +1330,8 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="8"/>
@@ -1373,7 +1373,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="48">
-        <v>2</v>
+        <v>4.43</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="7"/>
@@ -1387,11 +1387,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="56">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
       <c r="G7" s="12"/>
@@ -1403,11 +1403,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="51">
         <f>290*(10^(C6/10)-1)</f>
-        <v>169.61902581372294</v>
-      </c>
-      <c r="D8" s="53"/>
+        <v>514.26283034903372</v>
+      </c>
+      <c r="D8" s="51"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
       <c r="G8" s="12"/>
@@ -1419,11 +1419,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="61">
         <f>C5-10*LOG(C8)</f>
-        <v>7.7052543543729222</v>
-      </c>
-      <c r="D9" s="54"/>
+        <v>2.8881486428024701</v>
+      </c>
+      <c r="D9" s="61"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
       <c r="G9" s="12"/>
@@ -1473,11 +1473,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="51">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
       <c r="G12" s="12"/>
@@ -1489,11 +1489,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="12"/>
@@ -1507,11 +1507,11 @@
       </c>
       <c r="C14" s="31">
         <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>69.03755109901897</v>
+        <v>64.220445387448535</v>
       </c>
       <c r="D14" s="31">
         <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>85.424529777729049</v>
+        <v>80.607424066158615</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
@@ -1524,10 +1524,10 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="52">
         <v>0.44</v>
       </c>
-      <c r="D15" s="64"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="37" t="s">
         <v>45</v>
       </c>
@@ -1541,10 +1541,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -1555,10 +1555,10 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="54">
         <v>5</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
         <v>46</v>
@@ -1572,10 +1572,10 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="62">
         <v>5</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
         <v>46</v>
@@ -1590,7 +1590,7 @@
         <v>9</v>
       </c>
       <c r="C19" s="48">
-        <v>2</v>
+        <v>3.73</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="4"/>
@@ -1604,11 +1604,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="59">
+      <c r="C20" s="64">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="60"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
       <c r="G20" s="12"/>
@@ -1620,11 +1620,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="53">
+      <c r="C21" s="51">
         <f>290*(10^(C19/10)-1)</f>
-        <v>169.61902581372294</v>
-      </c>
-      <c r="D21" s="53"/>
+        <v>394.53868762236738</v>
+      </c>
+      <c r="D21" s="51"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
       <c r="G21" s="12"/>
@@ -1636,11 +1636,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="57">
         <f>C18-(10*LOG(C21))</f>
-        <v>-17.294745645627078</v>
-      </c>
-      <c r="D22" s="50"/>
+        <v>-20.960895956242979</v>
+      </c>
+      <c r="D22" s="58"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
       <c r="G22" s="12"/>
@@ -1708,11 +1708,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D26" s="52"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
       <c r="G26" s="12"/>
@@ -1726,11 +1726,11 @@
       </c>
       <c r="C27" s="31">
         <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>17.047851055658782</v>
+        <v>13.381700745042906</v>
       </c>
       <c r="D27" s="32">
         <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>33.434829734368861</v>
+        <v>29.768679423752985</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="13"/>
@@ -1857,15 +1857,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -1878,6 +1869,15 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1889,7 +1889,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,10 +1913,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="62"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1928,7 +1928,7 @@
       <c r="C2" s="48">
         <v>2.4</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="6" t="s">
         <v>47</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="57"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="66"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
@@ -1997,11 +1997,11 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="56">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="56"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
     </row>
@@ -2012,11 +2012,11 @@
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="51">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="53"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
     </row>
@@ -2027,11 +2027,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="61">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="54"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
     </row>
@@ -2079,11 +2079,11 @@
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="51">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
     </row>
@@ -2094,11 +2094,11 @@
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="51">
+      <c r="C13" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
     </row>
@@ -2129,7 +2129,7 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="63">
+      <c r="C15" s="52">
         <v>2.4</v>
       </c>
       <c r="D15" s="67"/>
@@ -2145,10 +2145,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="58"/>
+      <c r="D16" s="55"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -2159,10 +2159,10 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="54">
         <v>5</v>
       </c>
-      <c r="D17" s="58"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
         <v>46</v>
@@ -2175,10 +2175,10 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="62">
         <v>5</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
         <v>46</v>
@@ -2206,11 +2206,11 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="59">
+      <c r="C20" s="64">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="60"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
     </row>
@@ -2221,11 +2221,11 @@
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="53">
+      <c r="C21" s="51">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
@@ -2236,11 +2236,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="57">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="50"/>
+      <c r="D22" s="58"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
     </row>
@@ -2304,11 +2304,11 @@
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="59">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D26" s="52"/>
+      <c r="D26" s="60"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
     </row>
@@ -2511,6 +2511,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C25:D25"/>
@@ -2526,12 +2532,6 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Just some tweaks to get our budget more like IARU
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="-15" windowWidth="8070" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="4" r:id="rId1"/>
@@ -14,18 +14,20 @@
   <definedNames>
     <definedName name="alt">Intro!$C$5</definedName>
     <definedName name="c_">Intro!$C$4</definedName>
+    <definedName name="GSTP">Intro!$C$9</definedName>
     <definedName name="k">Intro!$C$3</definedName>
     <definedName name="radEarth">Intro!$C$2</definedName>
+    <definedName name="SCTP">Intro!$C$10</definedName>
     <definedName name="sdl">Intro!$C$7</definedName>
     <definedName name="udl">Intro!$C$6</definedName>
     <definedName name="ul">Intro!$C$8</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1" iterateCount="50"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
   <si>
     <t>Uplink Frequency</t>
   </si>
@@ -91,9 +93,6 @@
   </si>
   <si>
     <t>radEarth</t>
-  </si>
-  <si>
-    <t>Satellite Altitude</t>
   </si>
   <si>
     <t>alt</t>
@@ -228,6 +227,30 @@
   </si>
   <si>
     <t>J/K</t>
+  </si>
+  <si>
+    <t>Ground Station Antenna</t>
+  </si>
+  <si>
+    <t>Ground Station Losses</t>
+  </si>
+  <si>
+    <t>S/C Transmit Power</t>
+  </si>
+  <si>
+    <t>GS Transmit Power</t>
+  </si>
+  <si>
+    <t>S/C Altitude</t>
+  </si>
+  <si>
+    <t>GSTP</t>
+  </si>
+  <si>
+    <t>SCTP</t>
+  </si>
+  <si>
+    <t>S/C Losses</t>
   </si>
 </sst>
 </file>
@@ -279,7 +302,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -682,11 +705,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -779,65 +824,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,12 +1214,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
@@ -1173,93 +1232,121 @@
         <v>6378135</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="42">
         <f>1.380658E-23</f>
         <v>1.3806580000000001E-23</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="42">
         <v>299792400</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="C5" s="42">
         <v>300000</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="42">
         <f>100*1000</f>
         <v>100000</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C7" s="42">
         <v>1000000</v>
       </c>
       <c r="D7" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="42">
         <v>4000</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="71">
+        <v>100</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="71">
+        <v>5</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1273,15 +1360,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:D20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1289,7 +1376,7 @@
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="38" t="s">
         <v>1</v>
@@ -1300,458 +1387,454 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="63"/>
       <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="49">
         <v>0.44</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="49">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="J3" s="49"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="48">
-        <v>100</v>
-      </c>
-      <c r="D4" s="48"/>
+      <c r="C4" s="49">
+        <f>10*LOG(GSTP)</f>
+        <v>20</v>
+      </c>
+      <c r="D4" s="49"/>
       <c r="E4" s="6"/>
       <c r="F4" s="36"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48">
-        <v>30</v>
-      </c>
-      <c r="D5" s="48"/>
+      <c r="C5" s="49">
+        <v>15</v>
+      </c>
+      <c r="D5" s="49"/>
       <c r="E5" s="7"/>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="48">
-        <v>4.43</v>
-      </c>
-      <c r="D6" s="48"/>
+      <c r="C6" s="49">
+        <v>3.6</v>
+      </c>
+      <c r="D6" s="49"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56">
-        <f>10*LOG(C4)</f>
-        <v>20</v>
-      </c>
-      <c r="D7" s="56"/>
+      <c r="C7" s="58">
+        <f>C4+C5-C6</f>
+        <v>31.4</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="51">
-        <f>290*(10^(C6/10)-1)</f>
-        <v>514.26283034903372</v>
-      </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="14"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="58">
+        <v>2.6</v>
+      </c>
+      <c r="D8" s="59"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>15</v>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="61">
-        <f>C5-10*LOG(C8)</f>
-        <v>2.8881486428024701</v>
-      </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C9" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D9" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="8"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>22+20*LOG10((C9*1000)/C2)</f>
+        <v>155.06035024337962</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="54">
+        <f>290*(10^(C6/10)-1)</f>
+        <v>374.35161930265423</v>
+      </c>
+      <c r="D11" s="54"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="7"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="24">
-        <f>20*LOG((C10*1000))</f>
-        <v>125.92940377310335</v>
-      </c>
-      <c r="D11" s="24">
-        <f>20*LOG((D10*1000))</f>
-        <v>109.54242509439325</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="51">
+      <c r="C13" s="54">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="59">
-        <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
-        <v>-376.15135396075277</v>
-      </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="30" t="s">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="31">
-        <f>C7+C9-C13-C11-(20*LOG(C2*10^9))-C12</f>
-        <v>64.220445387448535</v>
-      </c>
-      <c r="D14" s="31">
-        <f>C7+C9-C13-D11-(20*LOG(C2*10^9))-C12</f>
-        <v>80.607424066158615</v>
-      </c>
+      <c r="C14" s="52">
+        <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
+        <v>-376.15135396075277</v>
+      </c>
+      <c r="D14" s="53"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+    <row r="15" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="31" t="e">
+        <f>C7+#REF!-C14-#REF!-(20*LOG(C2*10^9))-C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D15" s="31" t="e">
+        <f>C7+#REF!-C14-#REF!-(20*LOG(C2*10^9))-C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C16" s="64">
         <v>0.44</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="37" t="s">
+      <c r="D16" s="65"/>
+      <c r="E16" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="59"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C18" s="58">
         <v>5</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="62">
-        <v>5</v>
-      </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="59"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="F18" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="56">
+        <v>5</v>
+      </c>
+      <c r="D19" s="57"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="49">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="60">
+        <f>10*LOG(C18)</f>
+        <v>6.9897000433601884</v>
+      </c>
+      <c r="D21" s="61"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="48">
-        <v>3.73</v>
-      </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="64">
-        <f>10*LOG(C17)</f>
-        <v>6.9897000433601884</v>
-      </c>
-      <c r="D20" s="65"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="51">
-        <f>290*(10^(C19/10)-1)</f>
-        <v>394.53868762236738</v>
-      </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="C22" s="54">
+        <f>290*(10^(C20/10)-1)</f>
+        <v>217.45553970115063</v>
+      </c>
+      <c r="D22" s="54"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="57">
-        <f>C18-(10*LOG(C21))</f>
-        <v>-20.960895956242979</v>
-      </c>
-      <c r="D22" s="58"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="C23" s="50">
+        <f>C19-(10*LOG(C22))</f>
+        <v>-18.373704758367012</v>
+      </c>
+      <c r="D23" s="51"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C24" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(0))^2)^(1/2)-SIN(0)))/1000</f>
         <v>1979.1111641340412</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D24" s="23">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS(90)))^2)^(1/2)-SIN(RADIANS(90))))/1000</f>
         <v>300.00000000000011</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="24">
-        <f>20*LOG((C23*1000))</f>
-        <v>125.92940377310335</v>
-      </c>
-      <c r="D24" s="24">
-        <f>20*LOG((D23*1000))</f>
-        <v>109.54242509439325</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="36"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="24">
+        <f>20*LOG((C24*1000))</f>
+        <v>125.92940377310335</v>
+      </c>
+      <c r="D25" s="24">
+        <f>20*LOG((D24*1000))</f>
+        <v>109.54242509439325</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="49">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="D26" s="49"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="59">
+      <c r="C27" s="52">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="30" t="s">
+      <c r="D27" s="53"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="31">
-        <f>C20+C22-C26-C24-(20*LOG(C15*10^9))-C25</f>
-        <v>13.381700745042906</v>
-      </c>
-      <c r="D27" s="32">
-        <f>C20+C22-C26-D24-(20*LOG(C15*10^9))-C25</f>
-        <v>29.768679423752985</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="8"/>
+      <c r="C28" s="31">
+        <f>C21+C23-C27-C25-(20*LOG(C16*10^9))-C26</f>
+        <v>15.968891942918845</v>
+      </c>
+      <c r="D28" s="32">
+        <f>C21+C23-C27-D25-(20*LOG(C16*10^9))-C26</f>
+        <v>32.355870621628924</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1761,6 +1844,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
@@ -1769,7 +1853,6 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
@@ -1781,12 +1864,13 @@
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
@@ -1795,10 +1879,9 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="27"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -1816,7 +1899,7 @@
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="27"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1825,7 +1908,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1843,7 +1926,7 @@
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1852,32 +1935,42 @@
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
       <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="E42" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+  <mergeCells count="22">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C2:D2"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C15:D15"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1913,10 +2006,10 @@
       <c r="D1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="50"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
@@ -1925,15 +2018,15 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="48">
+      <c r="C2" s="49">
         <v>2.4</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" s="12"/>
     </row>
@@ -1942,23 +2035,23 @@
         <v>14</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="66"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="67"/>
       <c r="E3" s="7"/>
       <c r="F3" s="35"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="49">
         <v>100</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="6"/>
       <c r="F4" s="36"/>
     </row>
@@ -1969,24 +2062,24 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="49">
         <v>30</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="7"/>
       <c r="F5" s="35"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="49">
         <v>2</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="7"/>
       <c r="F6" s="14"/>
     </row>
@@ -1997,26 +2090,26 @@
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="66">
         <f>10*LOG(C4)</f>
         <v>20</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="6"/>
       <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="54">
         <f>290*(10^(C6/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D8" s="51"/>
+      <c r="D8" s="54"/>
       <c r="E8" s="4"/>
       <c r="F8" s="14"/>
     </row>
@@ -2027,11 +2120,11 @@
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="61">
+      <c r="C9" s="55">
         <f>C5-10*LOG(C8)</f>
         <v>7.7052543543729222</v>
       </c>
-      <c r="D9" s="61"/>
+      <c r="D9" s="55"/>
       <c r="E9" s="7"/>
       <c r="F9" s="36"/>
     </row>
@@ -2056,7 +2149,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -2074,37 +2167,37 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="54">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="7"/>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="59">
+      <c r="C13" s="52">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="30" t="s">
         <v>9</v>
@@ -2129,15 +2222,15 @@
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="64">
         <v>2.4</v>
       </c>
-      <c r="D15" s="67"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2145,10 +2238,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="55"/>
+      <c r="C16" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="59"/>
       <c r="E16" s="4"/>
       <c r="F16" s="14"/>
     </row>
@@ -2159,13 +2252,13 @@
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="58">
         <v>5</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="59"/>
       <c r="E17" s="7"/>
       <c r="F17" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2175,26 +2268,26 @@
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="62">
+      <c r="C18" s="56">
         <v>5</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="7"/>
       <c r="F18" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="49">
         <v>2</v>
       </c>
-      <c r="D19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="4"/>
       <c r="F19" s="8"/>
       <c r="G19" s="12"/>
@@ -2206,26 +2299,26 @@
       <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="64">
+      <c r="C20" s="60">
         <f>10*LOG(C17)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D20" s="65"/>
+      <c r="D20" s="61"/>
       <c r="E20" s="7"/>
       <c r="F20" s="36"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="54">
         <f>290*(10^(C19/10)-1)</f>
         <v>169.61902581372294</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
@@ -2236,11 +2329,11 @@
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="50">
         <f>C18-(10*LOG(C21))</f>
         <v>-17.294745645627078</v>
       </c>
-      <c r="D22" s="58"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="6"/>
       <c r="F22" s="36"/>
     </row>
@@ -2264,7 +2357,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>9</v>
@@ -2282,39 +2375,39 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="49">
         <f>10*LOG(sdl)</f>
         <v>60</v>
       </c>
-      <c r="D25" s="48"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="7"/>
       <c r="F25" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="59">
+      <c r="C26" s="52">
         <f>20*LOG(4*PI()/c_)+10*LOG(k)</f>
         <v>-376.15135396075277</v>
       </c>
-      <c r="D26" s="60"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="7"/>
       <c r="F26" s="35"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>9</v>
@@ -2511,12 +2604,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C25:D25"/>
@@ -2532,6 +2619,12 @@
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished S-Band Link Budget I think
Have to check if there are any loss differences between UHF and S-Band
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12975" activeTab="1"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -679,7 +679,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -716,9 +716,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,9 +739,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyFont="1" applyBorder="1"/>
@@ -776,16 +770,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -817,7 +803,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -830,7 +828,151 @@
     <cellStyle name="UP=Down? Yes" xfId="2"/>
     <cellStyle name="Yay" xfId="4"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="57"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="57"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="57"/>
+          <bgColor indexed="17"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="16"/>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1441,12 +1583,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1458,7 +1600,7 @@
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="47">
         <v>6378135</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -1475,7 +1617,7 @@
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="47">
         <v>-228.6</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -1489,7 +1631,7 @@
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="47">
         <v>299792400</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -1503,7 +1645,7 @@
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="48">
         <v>300000</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1511,27 +1653,27 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="55">
-        <v>0</v>
+      <c r="C6" s="49">
+        <v>38</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="49">
         <v>440</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -1539,13 +1681,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="44" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="49">
         <v>440</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1559,7 +1701,7 @@
       <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="48">
         <f>100*1000</f>
         <v>100000</v>
       </c>
@@ -1568,13 +1710,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="44" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C10" s="49">
         <v>2.4</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1582,13 +1724,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="55">
+      <c r="C11" s="49">
         <v>2.4</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -1602,7 +1744,7 @@
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="48">
         <v>1000000</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -1616,7 +1758,7 @@
       <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="48">
         <v>4000</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -1630,7 +1772,7 @@
       <c r="B14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="50">
         <v>100</v>
       </c>
       <c r="D14" s="16" t="s">
@@ -1638,13 +1780,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="44" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="55">
+      <c r="C15" s="49">
         <v>15</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -1652,14 +1794,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="45" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="57">
-        <v>3.6</v>
+      <c r="C16" s="51">
+        <v>2</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>41</v>
@@ -1669,10 +1811,10 @@
       <c r="A17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="58">
+      <c r="C17" s="52">
         <v>0.2</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -1686,7 +1828,7 @@
       <c r="B18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="53">
         <v>5</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -1700,7 +1842,7 @@
       <c r="B19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="60">
+      <c r="C19" s="54">
         <v>5</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1714,7 +1856,7 @@
       <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="60">
+      <c r="C20" s="54">
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -1725,10 +1867,10 @@
       <c r="A21" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="58">
+      <c r="C21" s="52">
         <v>0.6</v>
       </c>
       <c r="D21" s="18" t="s">
@@ -1742,7 +1884,7 @@
       <c r="B22" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="60">
+      <c r="C22" s="54">
         <v>261</v>
       </c>
       <c r="D22" s="18" t="s">
@@ -1756,7 +1898,7 @@
       <c r="B23" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="60">
+      <c r="C23" s="54">
         <v>510</v>
       </c>
       <c r="D23" s="18" t="s">
@@ -1770,7 +1912,7 @@
       <c r="B24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="60">
+      <c r="C24" s="54">
         <v>4.5999999999999996</v>
       </c>
       <c r="D24" s="18" t="s">
@@ -1784,7 +1926,7 @@
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="58">
+      <c r="C25" s="52">
         <v>0.2</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -1795,10 +1937,10 @@
       <c r="A26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="58">
+      <c r="C26" s="52">
         <v>0.4</v>
       </c>
       <c r="D26" s="18" t="s">
@@ -1809,13 +1951,13 @@
       <c r="A27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="61">
+      <c r="C27" s="55">
         <v>0.6</v>
       </c>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="36" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1834,8 +1976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,367 +1992,367 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="30"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23">
-        <f>udf</f>
+      <c r="C2" s="22">
+        <f>uuf</f>
         <v>440</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="30" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <f>10*LOG(GSTP)</f>
         <v>20</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <f>GSG</f>
         <v>15</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <f>GSL</f>
-        <v>3.6</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <f>C3+C4-C5</f>
-        <v>31.4</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <f>GSPL</f>
         <v>0.2</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="34"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <f>loss</f>
         <v>0.2</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="34"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="22">
         <f>AIL</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="34"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="22">
         <f>UIS</f>
         <v>0.4</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="34"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <v>1979</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="34"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="27">
         <f>22+20*LOG10((C11*1000)/(c_/(uuf*10^6)))</f>
         <v>151.26155703572783</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="34"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-125.26155703572783</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="34"/>
+        <v>-123.66155703572784</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="27">
         <f>SCG-SCL-10*LOG(SSNT)</f>
         <v>-21.166405073382808</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="27">
         <f>C13-C7-k+C14</f>
-        <v>81.972037890889354</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="34"/>
+        <v>83.572037890889348</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="41">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="34"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="42">
+      <c r="B17" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="40">
         <f>C15-C16</f>
-        <v>45.951437977609729</v>
+        <v>47.551437977609723</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="34"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="41"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="35"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="39"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="22">
         <f>udf</f>
         <v>440</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>56</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="28">
         <f>LOG(SCTP)</f>
         <v>0.69897000433601886</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="39"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="4"/>
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="22">
         <f>SCG</f>
         <v>5</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="22">
         <f>SCL</f>
         <v>2</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="34"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="27">
         <f>C20+C21-C22</f>
         <v>3.6989700043360187</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="34"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="32"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>90</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="27">
         <f>SCPL</f>
         <v>0.6</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="34"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="32"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="19" t="s">
@@ -2220,149 +2362,149 @@
         <f>loss</f>
         <v>0.2</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="62">
+      <c r="C26" s="56">
         <f>AIL</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="34"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="27">
         <f>DIS</f>
         <v>0.6</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(del))^2)^(1/2)-SIN(del)))/1000</f>
-        <v>1979.1111641340412</v>
-      </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36"/>
+        <v>846.51401891404282</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="27">
         <f>22+20*LOG10((C28*1000)/(c_/(udf*10^6)))</f>
-        <v>151.26204492470325</v>
-      </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
+        <v>143.88532424660877</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="34"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="27">
         <f>C23-SUM(C24:C27,C29)</f>
-        <v>-153.56307492036723</v>
-      </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="34"/>
+        <v>-146.18635424227276</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="32"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="24" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="27">
         <f>GSG-GSL-10*LOG(GSNT)</f>
-        <v>-15.675701760979363</v>
-      </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="34"/>
+        <v>-14.075701760979364</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="27">
         <f>C30-C24-k+C31</f>
-        <v>58.761223318653407</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="34"/>
+        <v>67.737943996747873</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="32"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="41">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="34"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="23" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="40">
         <f>C32-C33</f>
-        <v>8.761223318653407</v>
-      </c>
-      <c r="D34" s="35"/>
-      <c r="E34" s="34"/>
+        <v>17.737943996747873</v>
+      </c>
+      <c r="D34" s="33"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -2370,18 +2512,18 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2395,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,400 +2553,511 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="52"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="22">
+        <f>suf</f>
+        <v>2.4</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="22">
+        <f>10*LOG(GSTP)</f>
+        <v>20</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="22">
+        <f>GSG</f>
+        <v>15</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
+      <c r="C5" s="22">
+        <f>GSL</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="22">
+        <f>C3+C4-C5</f>
+        <v>33</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>90</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
+      <c r="C7" s="22">
+        <f>GSPL</f>
+        <v>0.2</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="34"/>
+      <c r="C8" s="22">
+        <f>loss</f>
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="34"/>
+      <c r="C9" s="22">
+        <f>AIL</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="34"/>
+      <c r="C10" s="22">
+        <f>UIS</f>
+        <v>0.4</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="34"/>
+      <c r="C11" s="25">
+        <v>1979</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="34"/>
+      <c r="C12" s="27">
+        <f>22+20*LOG10((C11*1000)/(c_/(suf*10^9)))</f>
+        <v>165.99672834023619</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="34"/>
+      <c r="C13" s="27">
+        <f>C6-SUM(C7:C10,C12)</f>
+        <v>-138.39672834023619</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>66</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="34"/>
+      <c r="C14" s="27">
+        <f>SCG-SCL-10*LOG(SSNT)</f>
+        <v>-21.166405073382808</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="39"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="C15" s="27">
+        <f>C13-C7-k+C14</f>
+        <v>68.836866586381007</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="37"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="34"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="C16" s="41">
+        <f>10*LOG(ul)</f>
+        <v>36.020599913279625</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="23" t="s">
         <v>71</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="39"/>
+      <c r="C17" s="40">
+        <f>C15-C16</f>
+        <v>32.816266673101381</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="50"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="46"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
+      <c r="C19" s="22">
+        <f>sdf</f>
+        <v>2.4</v>
+      </c>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="34"/>
+      <c r="C20" s="56">
+        <f>10*LOG(SCTP)</f>
+        <v>6.9897000433601884</v>
+      </c>
+      <c r="D20" s="33"/>
+      <c r="E20" s="32"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="34"/>
+      <c r="C21" s="22">
+        <f>SCG</f>
+        <v>5</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="24" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
+      <c r="C22" s="22">
+        <f>SCL</f>
+        <v>2</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="34"/>
+      <c r="C23" s="27">
+        <f>C20+C21-C22</f>
+        <v>9.9897000433601875</v>
+      </c>
+      <c r="D23" s="33"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>90</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="C24" s="27">
+        <f>GSPL</f>
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>89</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
+      <c r="C25" s="3">
+        <f>loss</f>
+        <v>0.2</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="34"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="24" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36"/>
+      <c r="C26" s="56">
+        <f>AIL</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="24" t="s">
         <v>88</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="34"/>
+      <c r="C27" s="27">
+        <f>DIS</f>
+        <v>0.6</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B28" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="34"/>
+      <c r="C28" s="25">
+        <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(del))^2)^(1/2)-SIN(del)))/1000</f>
+        <v>846.51401891404282</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="34"/>
+      <c r="C29" s="27">
+        <f>22+20*LOG10((C28*1000)/(c_/(sdf*10^9)))</f>
+        <v>158.62049555111713</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="34"/>
+      <c r="C30" s="27">
+        <f>C23-SUM(C24:C27,C29)</f>
+        <v>-154.23079550775694</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="32"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="24" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="34"/>
+      <c r="C31" s="27">
+        <f>GSG-GSL-10*LOG(GSNT)</f>
+        <v>-14.075701760979364</v>
+      </c>
+      <c r="D31" s="33"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="34"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="C32" s="27">
+        <f>C30-C24-k+C31</f>
+        <v>60.093502731263705</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="34"/>
-    </row>
-    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
+      <c r="C33" s="41">
+        <f>10*LOG(sdl)</f>
+        <v>60</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="23" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="34"/>
+      <c r="C34" s="40">
+        <f>C32-C33</f>
+        <v>9.3502731263704675E-2</v>
+      </c>
+      <c r="D34" s="33"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="D1:E1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Added initial formula for BER, need to find out Q
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -1977,7 +1977,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,7 +2252,10 @@
         <v>74</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="39"/>
+      <c r="C18" s="39">
+        <f>1*SQRT(2*0.68*C17)</f>
+        <v>8.0417632176997866</v>
+      </c>
       <c r="E18" s="36"/>
       <c r="F18" s="33"/>
     </row>
@@ -2502,7 +2505,10 @@
         <v>74</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
+      <c r="C35" s="39">
+        <f>1*SQRT(2*0.68*C34)</f>
+        <v>4.911578548244659</v>
+      </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
     </row>
@@ -2538,7 +2544,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2805,10 @@
         <v>74</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="39"/>
+      <c r="C18" s="39">
+        <f>1*SQRT(2*0.68*C17)</f>
+        <v>6.6805780195592268</v>
+      </c>
       <c r="D18" s="35"/>
       <c r="E18" s="46"/>
     </row>
@@ -3033,7 +3042,10 @@
         <v>74</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
+      <c r="C35" s="39">
+        <f>1*SQRT(2*0.68*C34)</f>
+        <v>0.35660021665534414</v>
+      </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
     </row>

</xml_diff>

<commit_message>
Adjusted the bit error rate formula
Might be more right
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -759,7 +759,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -818,6 +817,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel Built-in Normal" xfId="6"/>
@@ -828,103 +828,7 @@
     <cellStyle name="UP=Down? Yes" xfId="2"/>
     <cellStyle name="Yay" xfId="4"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="57"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="57"/>
-          <bgColor indexed="17"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="16"/>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b/>
@@ -1583,12 +1487,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1600,7 +1504,7 @@
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="46">
         <v>6378135</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -1617,7 +1521,7 @@
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="46">
         <v>-228.6</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -1631,7 +1535,7 @@
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="46">
         <v>299792400</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -1645,7 +1549,7 @@
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="47">
         <v>300000</v>
       </c>
       <c r="D5" s="14" t="s">
@@ -1653,13 +1557,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="48">
         <v>38</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -1667,13 +1571,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="48">
         <v>440</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -1681,13 +1585,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="48">
         <v>440</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -1701,7 +1605,7 @@
       <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="47">
         <f>100*1000</f>
         <v>100000</v>
       </c>
@@ -1710,13 +1614,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="48">
         <v>2.4</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1724,13 +1628,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="48">
         <v>2.4</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -1744,7 +1648,7 @@
       <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="48">
+      <c r="C12" s="47">
         <v>1000000</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -1758,7 +1662,7 @@
       <c r="B13" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="47">
         <v>4000</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -1772,7 +1676,7 @@
       <c r="B14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="50">
+      <c r="C14" s="49">
         <v>100</v>
       </c>
       <c r="D14" s="16" t="s">
@@ -1780,13 +1684,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="48">
         <v>15</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -1794,13 +1698,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="51">
+      <c r="C16" s="50">
         <v>2</v>
       </c>
       <c r="D16" s="17" t="s">
@@ -1814,7 +1718,7 @@
       <c r="B17" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="51">
         <v>0.2</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -1828,7 +1732,7 @@
       <c r="B18" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="53">
+      <c r="C18" s="52">
         <v>5</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -1842,7 +1746,7 @@
       <c r="B19" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="53">
         <v>5</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1856,7 +1760,7 @@
       <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="53">
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
@@ -1870,7 +1774,7 @@
       <c r="B21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="52">
+      <c r="C21" s="51">
         <v>0.6</v>
       </c>
       <c r="D21" s="18" t="s">
@@ -1884,7 +1788,7 @@
       <c r="B22" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="53">
         <v>261</v>
       </c>
       <c r="D22" s="18" t="s">
@@ -1898,7 +1802,7 @@
       <c r="B23" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="53">
         <v>510</v>
       </c>
       <c r="D23" s="18" t="s">
@@ -1912,7 +1816,7 @@
       <c r="B24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="53">
         <v>4.5999999999999996</v>
       </c>
       <c r="D24" s="18" t="s">
@@ -1926,7 +1830,7 @@
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="52">
+      <c r="C25" s="51">
         <v>0.2</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -1940,7 +1844,7 @@
       <c r="B26" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="52">
+      <c r="C26" s="51">
         <v>0.4</v>
       </c>
       <c r="D26" s="18" t="s">
@@ -1954,7 +1858,7 @@
       <c r="B27" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="54">
         <v>0.6</v>
       </c>
       <c r="D27" s="36" t="s">
@@ -1977,7 +1881,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,10 +1902,10 @@
       <c r="C1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2224,7 +2128,7 @@
       <c r="B16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="40">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
@@ -2239,7 +2143,7 @@
       <c r="B17" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="39">
         <f>C15-C16</f>
         <v>47.551437977609723</v>
       </c>
@@ -2252,9 +2156,9 @@
         <v>74</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="39">
-        <f>1*SQRT(2*0.68*C17)</f>
-        <v>8.0417632176997866</v>
+      <c r="C18" s="60">
+        <f>0.5*SQRT(C17)</f>
+        <v>3.4478775347164565</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="33"/>
@@ -2376,7 +2280,7 @@
       <c r="B26" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="55">
         <f>AIL</f>
         <v>4.5999999999999996</v>
       </c>
@@ -2479,7 +2383,7 @@
       <c r="B33" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="40">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
@@ -2493,7 +2397,7 @@
       <c r="B34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="39">
         <f>C32-C33</f>
         <v>17.737943996747873</v>
       </c>
@@ -2505,9 +2409,9 @@
         <v>74</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="39">
-        <f>1*SQRT(2*0.68*C34)</f>
-        <v>4.911578548244659</v>
+      <c r="C35" s="60">
+        <f>0.5*SQRT(C34)</f>
+        <v>2.1058219296006415</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
@@ -2518,18 +2422,18 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2544,7 +2448,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,10 +2469,10 @@
       <c r="C1" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="60"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2779,7 +2683,7 @@
       <c r="B16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="40">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
@@ -2793,7 +2697,7 @@
       <c r="B17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="39">
         <f>C15-C16</f>
         <v>32.816266673101381</v>
       </c>
@@ -2805,12 +2709,12 @@
         <v>74</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="39">
-        <f>1*SQRT(2*0.68*C17)</f>
-        <v>6.6805780195592268</v>
+      <c r="C18" s="60">
+        <f>0.5*SQRT(C17)</f>
+        <v>2.8642741957213778</v>
       </c>
       <c r="D18" s="35"/>
-      <c r="E18" s="46"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
@@ -2823,8 +2727,8 @@
         <f>sdf</f>
         <v>2.4</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2834,7 +2738,7 @@
       <c r="B20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="55">
         <f>10*LOG(SCTP)</f>
         <v>6.9897000433601884</v>
       </c>
@@ -2918,7 +2822,7 @@
       <c r="B26" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="55">
         <f>AIL</f>
         <v>4.5999999999999996</v>
       </c>
@@ -3016,7 +2920,7 @@
       <c r="B33" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="40">
         <f>10*LOG(sdl)</f>
         <v>60</v>
       </c>
@@ -3030,7 +2934,7 @@
       <c r="B34" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="39">
         <f>C32-C33</f>
         <v>9.3502731263704675E-2</v>
       </c>
@@ -3042,9 +2946,9 @@
         <v>74</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="39">
-        <f>1*SQRT(2*0.68*C34)</f>
-        <v>0.35660021665534414</v>
+      <c r="C35" s="60">
+        <f>0.5*SQRT(C34)</f>
+        <v>0.15289108154475908</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
@@ -3055,18 +2959,18 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
The right BER formula finally
Thanks Swartwout!
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990" activeTab="2"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -389,9 +389,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -679,7 +681,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
@@ -817,7 +819,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel Built-in Normal" xfId="6"/>
@@ -1473,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1881,7 +1884,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,9 +2159,9 @@
         <v>74</v>
       </c>
       <c r="B18" s="22"/>
-      <c r="C18" s="60">
-        <f>0.5*SQRT(C17)</f>
-        <v>3.4478775347164565</v>
+      <c r="C18" s="61">
+        <f>0.5*ERFC(2*(C17/SQRT(2)))</f>
+        <v>0</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="33"/>
@@ -2409,9 +2412,9 @@
         <v>74</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="60">
-        <f>0.5*SQRT(C34)</f>
-        <v>2.1058219296006415</v>
+      <c r="C35" s="61">
+        <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
+        <v>5.7868402383453132E-276</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
@@ -2438,7 +2441,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -2447,15 +2450,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7109375" style="1"/>
@@ -2710,8 +2713,8 @@
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="60">
-        <f>0.5*SQRT(C17)</f>
-        <v>2.8642741957213778</v>
+        <f>0.5*ERFC(2*(C17/SQRT(2)))</f>
+        <v>0</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="45"/>
@@ -2947,8 +2950,8 @@
       </c>
       <c r="B35" s="22"/>
       <c r="C35" s="60">
-        <f>0.5*SQRT(C34)</f>
-        <v>0.15289108154475908</v>
+        <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
+        <v>0.4258281750122187</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>

</xml_diff>

<commit_message>
Found the minimum angle needed for s-band
this is the angle needed to close the link
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1601,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="47">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>15</v>
@@ -1752,7 +1752,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="49">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>41</v>
@@ -1812,7 +1812,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="52">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>41</v>
@@ -1872,7 +1872,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="52">
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>41</v>
@@ -1941,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="C5" s="58">
         <f>GSL</f>
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>96</v>
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C6" s="22">
         <f>C3+C4-C5</f>
-        <v>31.4</v>
+        <v>33</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="32"/>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="C9" s="22">
         <f>AIL</f>
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="C11" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>2574.5164594540856</v>
+        <v>1192.9918144524856</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="C12" s="27">
         <f>22+20*LOG10((C11*1000)/(c_/(uuf*10^6)))</f>
-        <v>153.54655460585923</v>
+        <v>146.86539042818674</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C13" s="27">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-127.54655460585923</v>
+        <v>-115.76539042818675</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="C14" s="27">
         <f>SCG-SCL-10*LOG(SSNT)</f>
-        <v>-21.166405073382808</v>
+        <v>-21.366405073382808</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="C15" s="27">
         <f>C13-C7-k+C14</f>
-        <v>79.687040320757959</v>
+        <v>91.268204498430435</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="C17" s="39">
         <f>C15-C16</f>
-        <v>43.666440407478333</v>
+        <v>55.24760458515081</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="32"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C22" s="58">
         <f>SCL</f>
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D22" s="55" t="s">
         <v>96</v>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C23" s="27">
         <f>C20+C21-C22</f>
-        <v>3.6989700043360187</v>
+        <v>3.4989700043360186</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C26" s="54">
         <f>AIL</f>
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="C28" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>2574.5164594540856</v>
+        <v>1192.9918144524856</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="34"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="C29" s="27">
         <f>22+20*LOG10((C28*1000)/(c_/(udf*10^6)))</f>
-        <v>153.54655460585923</v>
+        <v>146.86539042818674</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="34"/>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="C30" s="27">
         <f>C23-SUM(C24:C27,C29)</f>
-        <v>-156.0475846015232</v>
+        <v>-146.0664204238507</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="C31" s="27">
         <f>GSG-GSL-10*LOG(GSNT)</f>
-        <v>-15.675701760979363</v>
+        <v>-14.075701760979364</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="C32" s="27">
         <f>C30-C24-k+C31</f>
-        <v>56.276713637497437</v>
+        <v>67.857877815169928</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C34" s="39">
         <f>C32-C33</f>
-        <v>6.276713637497437</v>
+        <v>17.857877815169928</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
@@ -2473,7 +2473,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="59">
         <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
-        <v>1.9033489403159599E-36</v>
+        <v>1.1256132052109896E-279</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
@@ -2509,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C5" s="58">
         <f>GSL</f>
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>96</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C6" s="22">
         <f>C3+C4-C5</f>
-        <v>31.4</v>
+        <v>33</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="32"/>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="C9" s="22">
         <f>AIL</f>
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C11" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>2574.5164594540856</v>
+        <v>1192.9918144524856</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="C12" s="27">
         <f>22+20*LOG10((C11*1000)/(c_/(suf*10^9)))</f>
-        <v>168.28172591036758</v>
+        <v>161.6005617326951</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="C13" s="27">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-142.28172591036758</v>
+        <v>-130.5005617326951</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="C14" s="27">
         <f>SCG-SCL-10*LOG(SSNT)</f>
-        <v>-21.166405073382808</v>
+        <v>-21.366405073382808</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="C15" s="27">
         <f>C13-C7-k+C14</f>
-        <v>64.951869016249617</v>
+        <v>76.533033193922094</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="37"/>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C17" s="39">
         <f>C15-C16</f>
-        <v>28.931269102969992</v>
+        <v>40.512433280642469</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="37"/>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="C22" s="58">
         <f>SCL</f>
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D22" s="55" t="s">
         <v>96</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C23" s="27">
         <f>C20+C21-C22</f>
-        <v>9.9897000433601875</v>
+        <v>9.7897000433601882</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="C26" s="54">
         <f>AIL</f>
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="34"/>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="C28" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>2574.5164594540856</v>
+        <v>1192.9918144524856</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="C29" s="27">
         <f>22+20*LOG10((C28*1000)/(c_/(sdf*10^9)))</f>
-        <v>168.28172591036758</v>
+        <v>161.6005617326951</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="C30" s="27">
         <f>C23-SUM(C24:C27,C29)</f>
-        <v>-164.09202586700741</v>
+        <v>-154.11086168933491</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="C31" s="27">
         <f>GSG-GSL-10*LOG(GSNT)</f>
-        <v>-15.675701760979363</v>
+        <v>-14.075701760979364</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="C32" s="27">
         <f>C30-C24-k+C31</f>
-        <v>48.632272372013233</v>
+        <v>60.213436549685731</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C34" s="39">
         <f>C32-C33</f>
-        <v>-11.367727627986767</v>
+        <v>0.21343654968573134</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
@@ -3018,7 +3018,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="59">
         <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
-        <v>1</v>
+        <v>0.33473587995436138</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>

</xml_diff>

<commit_message>
Looked at altitude of 300 km and 5 deg elevation
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1586,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="46">
-        <v>500000</v>
+        <v>300000</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>3</v>
@@ -1601,7 +1601,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="47">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>15</v>
@@ -1752,7 +1752,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="49">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>41</v>
@@ -1812,7 +1812,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="52">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>41</v>
@@ -1872,7 +1872,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="52">
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>41</v>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="C5" s="58">
         <f>GSL</f>
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>96</v>
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C6" s="22">
         <f>C3+C4-C5</f>
-        <v>33</v>
+        <v>31.4</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="32"/>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="C9" s="22">
         <f>AIL</f>
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="C11" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>1192.9918144524856</v>
+        <v>1499.8073057120612</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="C12" s="27">
         <f>22+20*LOG10((C11*1000)/(c_/(uuf*10^6)))</f>
-        <v>146.86539042818674</v>
+        <v>148.85335044682444</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C13" s="27">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-115.76539042818675</v>
+        <v>-120.35335044682444</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="C14" s="27">
         <f>SCG-SCL-10*LOG(SSNT)</f>
-        <v>-21.366405073382808</v>
+        <v>-21.166405073382808</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="C15" s="27">
         <f>C13-C7-k+C14</f>
-        <v>91.268204498430435</v>
+        <v>86.880244479792751</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="C17" s="39">
         <f>C15-C16</f>
-        <v>55.24760458515081</v>
+        <v>50.859644566513126</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="32"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C22" s="58">
         <f>SCL</f>
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D22" s="55" t="s">
         <v>96</v>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C23" s="27">
         <f>C20+C21-C22</f>
-        <v>3.4989700043360186</v>
+        <v>3.6989700043360187</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="C26" s="54">
         <f>AIL</f>
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
@@ -2374,7 +2374,7 @@
       </c>
       <c r="C28" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>1192.9918144524856</v>
+        <v>1499.8073057120612</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="34"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="C29" s="27">
         <f>22+20*LOG10((C28*1000)/(c_/(udf*10^6)))</f>
-        <v>146.86539042818674</v>
+        <v>148.85335044682444</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="34"/>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="C30" s="27">
         <f>C23-SUM(C24:C27,C29)</f>
-        <v>-146.0664204238507</v>
+        <v>-148.85438044248841</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="C31" s="27">
         <f>GSG-GSL-10*LOG(GSNT)</f>
-        <v>-14.075701760979364</v>
+        <v>-15.675701760979363</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="C32" s="27">
         <f>C30-C24-k+C31</f>
-        <v>67.857877815169928</v>
+        <v>63.469917796532229</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C34" s="39">
         <f>C32-C33</f>
-        <v>17.857877815169928</v>
+        <v>13.469917796532229</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
@@ -2473,7 +2473,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="59">
         <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
-        <v>1.1256132052109896E-279</v>
+        <v>3.7521395553574855E-160</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
@@ -2509,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C5" s="58">
         <f>GSL</f>
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>96</v>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="C6" s="22">
         <f>C3+C4-C5</f>
-        <v>33</v>
+        <v>31.4</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="32"/>
@@ -2650,7 +2650,7 @@
       </c>
       <c r="C9" s="22">
         <f>AIL</f>
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C11" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>1192.9918144524856</v>
+        <v>1499.8073057120612</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="C12" s="27">
         <f>22+20*LOG10((C11*1000)/(c_/(suf*10^9)))</f>
-        <v>161.6005617326951</v>
+        <v>163.58852175133279</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="C13" s="27">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-130.5005617326951</v>
+        <v>-135.08852175133279</v>
       </c>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="C14" s="27">
         <f>SCG-SCL-10*LOG(SSNT)</f>
-        <v>-21.366405073382808</v>
+        <v>-21.166405073382808</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="C15" s="27">
         <f>C13-C7-k+C14</f>
-        <v>76.533033193922094</v>
+        <v>72.145073175284409</v>
       </c>
       <c r="D15" s="33"/>
       <c r="E15" s="37"/>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="C17" s="39">
         <f>C15-C16</f>
-        <v>40.512433280642469</v>
+        <v>36.124473262004784</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="37"/>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="C22" s="58">
         <f>SCL</f>
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D22" s="55" t="s">
         <v>96</v>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C23" s="27">
         <f>C20+C21-C22</f>
-        <v>9.7897000433601882</v>
+        <v>9.9897000433601875</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="C26" s="54">
         <f>AIL</f>
-        <v>1.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D26" s="33"/>
       <c r="E26" s="34"/>
@@ -2922,7 +2922,7 @@
       </c>
       <c r="C28" s="25">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
-        <v>1192.9918144524856</v>
+        <v>1499.8073057120612</v>
       </c>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="C29" s="27">
         <f>22+20*LOG10((C28*1000)/(c_/(sdf*10^9)))</f>
-        <v>161.6005617326951</v>
+        <v>163.58852175133279</v>
       </c>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="C30" s="27">
         <f>C23-SUM(C24:C27,C29)</f>
-        <v>-154.11086168933491</v>
+        <v>-156.89882170797262</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="C31" s="27">
         <f>GSG-GSL-10*LOG(GSNT)</f>
-        <v>-14.075701760979364</v>
+        <v>-15.675701760979363</v>
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="C32" s="27">
         <f>C30-C24-k+C31</f>
-        <v>60.213436549685731</v>
+        <v>55.825476531048025</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C34" s="39">
         <f>C32-C33</f>
-        <v>0.21343654968573134</v>
+        <v>-4.1745234689519748</v>
       </c>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
@@ -3018,7 +3018,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="59">
         <f>0.5*ERFC(2*(C34/SQRT(2)))</f>
-        <v>0.33473587995436138</v>
+        <v>1</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>

</xml_diff>

<commit_message>
I don't know what i changed
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12405" activeTab="2"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
   <si>
     <t>Yes</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Affected by elevation angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1941,7 +1944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>41</v>
@@ -2509,7 +2512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created Inter-Satellite Link Budget
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12390" activeTab="1"/>
+    <workbookView xWindow="16380" yWindow="405" windowWidth="8430" windowHeight="12405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
   <si>
     <t>Yes</t>
   </si>
@@ -395,9 +395,6 @@
   </si>
   <si>
     <t>Affected by elevation angle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1942,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2095,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>41</v>
@@ -2512,7 +2509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Distance numbers & antenna improvements
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9720" windowHeight="7320"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1461,11 +1461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
@@ -1475,7 +1475,7 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>26</v>
       </c>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>31</v>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>33</v>
       </c>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>35</v>
       </c>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>38</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>41</v>
       </c>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>44</v>
       </c>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>48</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>50</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>52</v>
       </c>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>57</v>
       </c>
@@ -1823,7 +1823,7 @@
       </c>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1">
+    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>59</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>62</v>
       </c>
@@ -1855,7 +1855,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>64</v>
       </c>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>66</v>
       </c>
@@ -1900,9 +1900,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="28" customWidth="1"/>
@@ -1912,7 +1914,7 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>68</v>
@@ -1926,7 +1928,7 @@
       <c r="E1" s="59"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>71</v>
       </c>
@@ -1943,7 +1945,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="31"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>73</v>
       </c>
@@ -1958,7 +1960,7 @@
       <c r="E3" s="37"/>
       <c r="F3" s="31"/>
     </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1">
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>74</v>
       </c>
@@ -1973,7 +1975,7 @@
       <c r="E4" s="40"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>75</v>
       </c>
@@ -1990,7 +1992,7 @@
       <c r="E5" s="37"/>
       <c r="F5" s="31"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>77</v>
       </c>
@@ -2005,7 +2007,7 @@
       <c r="E6" s="37"/>
       <c r="F6" s="31"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>79</v>
       </c>
@@ -2020,7 +2022,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>80</v>
       </c>
@@ -2035,7 +2037,7 @@
       <c r="E8" s="37"/>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>81</v>
       </c>
@@ -2048,12 +2050,9 @@
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="37"/>
-      <c r="F9" s="31">
-        <f>k</f>
-        <v>-228.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>82</v>
       </c>
@@ -2066,12 +2065,9 @@
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="37"/>
-      <c r="F10" s="31">
-        <f>c_</f>
-        <v>299792400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>83</v>
       </c>
@@ -2086,7 +2082,7 @@
       <c r="E11" s="37"/>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
         <v>85</v>
       </c>
@@ -2101,7 +2097,7 @@
       <c r="E12" s="37"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>86</v>
       </c>
@@ -2116,7 +2112,7 @@
       <c r="E13" s="37"/>
       <c r="F13" s="31"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>87</v>
       </c>
@@ -2131,7 +2127,7 @@
       <c r="E14" s="37"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:6" ht="18">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>89</v>
       </c>
@@ -2146,7 +2142,7 @@
       <c r="E15" s="37"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>91</v>
       </c>
@@ -2161,7 +2157,7 @@
       <c r="E16" s="37"/>
       <c r="F16" s="31"/>
     </row>
-    <row r="17" spans="1:10" ht="18">
+    <row r="17" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="35" t="s">
         <v>92</v>
       </c>
@@ -2176,7 +2172,7 @@
       <c r="E17" s="37"/>
       <c r="F17" s="31"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>93</v>
       </c>
@@ -2188,7 +2184,7 @@
       <c r="E18" s="27"/>
       <c r="F18" s="39"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>94</v>
       </c>
@@ -2205,7 +2201,7 @@
       <c r="E19" s="34"/>
       <c r="F19" s="31"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>96</v>
       </c>
@@ -2221,7 +2217,7 @@
       <c r="F20" s="31"/>
       <c r="J20" s="31"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>74</v>
       </c>
@@ -2236,7 +2232,7 @@
       <c r="E21" s="53"/>
       <c r="F21" s="31"/>
     </row>
-    <row r="22" spans="1:10" ht="30">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>97</v>
       </c>
@@ -2253,7 +2249,7 @@
       <c r="E22" s="37"/>
       <c r="F22" s="31"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>77</v>
       </c>
@@ -2268,7 +2264,7 @@
       <c r="E23" s="37"/>
       <c r="F23" s="31"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>79</v>
       </c>
@@ -2283,7 +2279,7 @@
       <c r="E24" s="37"/>
       <c r="F24" s="31"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>80</v>
       </c>
@@ -2298,7 +2294,7 @@
       <c r="E25" s="37"/>
       <c r="F25" s="31"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>81</v>
       </c>
@@ -2313,7 +2309,7 @@
       <c r="E26" s="37"/>
       <c r="F26" s="31"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>82</v>
       </c>
@@ -2328,7 +2324,7 @@
       <c r="E27" s="37"/>
       <c r="F27" s="31"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>83</v>
       </c>
@@ -2343,7 +2339,7 @@
       <c r="E28" s="40"/>
       <c r="F28" s="31"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
         <v>85</v>
       </c>
@@ -2358,7 +2354,7 @@
       <c r="E29" s="40"/>
       <c r="F29" s="31"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
         <v>98</v>
       </c>
@@ -2373,7 +2369,7 @@
       <c r="E30" s="37"/>
       <c r="F30" s="31"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
         <v>87</v>
       </c>
@@ -2387,7 +2383,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="37"/>
     </row>
-    <row r="32" spans="1:10" ht="18">
+    <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>89</v>
       </c>
@@ -2401,7 +2397,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="37"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>91</v>
       </c>
@@ -2415,7 +2411,7 @@
       <c r="D33" s="39"/>
       <c r="E33" s="37"/>
     </row>
-    <row r="34" spans="1:5" ht="18">
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
         <v>92</v>
       </c>
@@ -2429,7 +2425,7 @@
       <c r="D34" s="39"/>
       <c r="E34" s="37"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>93</v>
       </c>
@@ -2474,7 +2470,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
@@ -2484,7 +2480,7 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>68</v>
@@ -2498,7 +2494,7 @@
       <c r="E1" s="59"/>
       <c r="F1" s="39"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>71</v>
       </c>
@@ -2515,7 +2511,7 @@
       <c r="E2" s="34"/>
       <c r="F2" s="31"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>73</v>
       </c>
@@ -2530,7 +2526,7 @@
       <c r="E3" s="40"/>
       <c r="F3" s="31"/>
     </row>
-    <row r="4" spans="1:11" ht="16.5" customHeight="1">
+    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>74</v>
       </c>
@@ -2544,7 +2540,7 @@
       <c r="D4" s="36"/>
       <c r="E4" s="37"/>
     </row>
-    <row r="5" spans="1:11" ht="30.75" customHeight="1">
+    <row r="5" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>75</v>
       </c>
@@ -2560,7 +2556,7 @@
       </c>
       <c r="E5" s="40"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>77</v>
       </c>
@@ -2574,7 +2570,7 @@
       <c r="D6" s="36"/>
       <c r="E6" s="37"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>79</v>
       </c>
@@ -2588,7 +2584,7 @@
       <c r="D7" s="39"/>
       <c r="E7" s="37"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>80</v>
       </c>
@@ -2602,7 +2598,7 @@
       <c r="D8" s="39"/>
       <c r="E8" s="37"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>81</v>
       </c>
@@ -2617,7 +2613,7 @@
       <c r="E9" s="37"/>
       <c r="G9" s="31"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>82</v>
       </c>
@@ -2632,7 +2628,7 @@
       <c r="E10" s="37"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>83</v>
       </c>
@@ -2646,7 +2642,7 @@
       <c r="D11" s="39"/>
       <c r="E11" s="37"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
         <v>85</v>
       </c>
@@ -2660,7 +2656,7 @@
       <c r="D12" s="39"/>
       <c r="E12" s="37"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>86</v>
       </c>
@@ -2674,7 +2670,7 @@
       <c r="D13" s="39"/>
       <c r="E13" s="37"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>87</v>
       </c>
@@ -2690,7 +2686,7 @@
       <c r="F14" s="31"/>
       <c r="K14" s="31"/>
     </row>
-    <row r="15" spans="1:11" ht="18">
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>89</v>
       </c>
@@ -2704,7 +2700,7 @@
       <c r="D15" s="39"/>
       <c r="E15" s="53"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>91</v>
       </c>
@@ -2718,7 +2714,7 @@
       <c r="D16" s="39"/>
       <c r="E16" s="37"/>
     </row>
-    <row r="17" spans="1:6" ht="18">
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="35" t="s">
         <v>92</v>
       </c>
@@ -2732,7 +2728,7 @@
       <c r="D17" s="31"/>
       <c r="E17" s="53"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>93</v>
       </c>
@@ -2743,7 +2739,7 @@
       </c>
       <c r="E18" s="56"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>94</v>
       </c>
@@ -2760,7 +2756,7 @@
       <c r="E19" s="57"/>
       <c r="F19" s="31"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>96</v>
       </c>
@@ -2774,7 +2770,7 @@
       <c r="D20" s="39"/>
       <c r="E20" s="37"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>74</v>
       </c>
@@ -2788,7 +2784,7 @@
       <c r="D21" s="39"/>
       <c r="E21" s="37"/>
     </row>
-    <row r="22" spans="1:6" ht="29.25" customHeight="1">
+    <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>97</v>
       </c>
@@ -2804,7 +2800,7 @@
       </c>
       <c r="E22" s="37"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>77</v>
       </c>
@@ -2818,7 +2814,7 @@
       <c r="D23" s="39"/>
       <c r="E23" s="37"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
         <v>79</v>
       </c>
@@ -2832,7 +2828,7 @@
       <c r="D24" s="36"/>
       <c r="E24" s="37"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="38" t="s">
         <v>80</v>
       </c>
@@ -2846,7 +2842,7 @@
       <c r="D25" s="39"/>
       <c r="E25" s="40"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="38" t="s">
         <v>81</v>
       </c>
@@ -2860,7 +2856,7 @@
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>82</v>
       </c>
@@ -2874,7 +2870,7 @@
       <c r="D27" s="39"/>
       <c r="E27" s="37"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>83</v>
       </c>
@@ -2888,7 +2884,7 @@
       <c r="D28" s="39"/>
       <c r="E28" s="37"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
         <v>85</v>
       </c>
@@ -2902,7 +2898,7 @@
       <c r="D29" s="39"/>
       <c r="E29" s="37"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
         <v>86</v>
       </c>
@@ -2916,7 +2912,7 @@
       <c r="D30" s="39"/>
       <c r="E30" s="37"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
         <v>87</v>
       </c>
@@ -2930,7 +2926,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="37"/>
     </row>
-    <row r="32" spans="1:6" ht="18">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>89</v>
       </c>
@@ -2944,7 +2940,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="37"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>91</v>
       </c>
@@ -2958,7 +2954,7 @@
       <c r="D33" s="39"/>
       <c r="E33" s="37"/>
     </row>
-    <row r="34" spans="1:5" ht="18">
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="35" t="s">
         <v>92</v>
       </c>
@@ -2972,7 +2968,7 @@
       <c r="D34" s="39"/>
       <c r="E34" s="37"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
Corrected GS transmit pwoer
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM1.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12990" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -1461,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,7 +1681,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="17">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>37</v>
@@ -1900,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1954,7 +1954,7 @@
       </c>
       <c r="C3" s="2">
         <f>10*LOG(GSTP)</f>
-        <v>20</v>
+        <v>16.989700043360187</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="37"/>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C6" s="2">
         <f>C3+C4-C5</f>
-        <v>31.4</v>
+        <v>28.389700043360186</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="37"/>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="C13" s="47">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-120.35335044682444</v>
+        <v>-123.36365040346425</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="37"/>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="C15" s="47">
         <f>C13-C7-k+C14</f>
-        <v>86.880244479792751</v>
+        <v>83.869944523152938</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="37"/>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="C17" s="50">
         <f>C15-C16</f>
-        <v>50.859644566513126</v>
+        <v>47.849344609873313</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="37"/>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="C3" s="2">
         <f>10*LOG(GSTP)</f>
-        <v>20</v>
+        <v>16.989700043360187</v>
       </c>
       <c r="D3" s="39"/>
       <c r="E3" s="40"/>
@@ -2565,7 +2565,7 @@
       </c>
       <c r="C6" s="2">
         <f>C3+C4-C5</f>
-        <v>31.4</v>
+        <v>28.389700043360186</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="37"/>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="C13" s="47">
         <f>C6-SUM(C7:C10,C12)</f>
-        <v>-135.08852175133279</v>
+        <v>-138.0988217079726</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="37"/>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="C15" s="47">
         <f>C13-C7-k+C14</f>
-        <v>72.145073175284409</v>
+        <v>69.134773218644597</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="53"/>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="C17" s="50">
         <f>C15-C16</f>
-        <v>36.124473262004784</v>
+        <v>33.114173305364972</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="53"/>

</xml_diff>